<commit_message>
Add pandas table for all methods
+ pandas table for * methods
* xlsx writing
* umo, main pyth
</commit_message>
<xml_diff>
--- a/Table.xlsx
+++ b/Table.xlsx
@@ -7,7 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Steepest Descent" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Найшвидшого спуску" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Спряжених градієнтів" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Ньютона" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Квазі-Ньютона (BFGS)" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1189,4 +1192,1914 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fun</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>grad</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>alpha</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>gnorm</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>iter</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>-14</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[-8.94427190999916, -8.94427190999916]</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12.64911064067352</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[-1.118033988749895, -1.118033988749895]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-20.25</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[4.192627457812106, -2.5155764746872635]</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6.708203932499369</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[-0.06987712429686832, -1.7469281074217107]</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>-23.6337890625</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[-0.8483519621666693, -1.9227127482310218]</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.096313728906054</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[-0.17592111956770198, -1.9872672009505883]</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-23.89653239026666</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>[0.6349190719216727, -0.5840871735123434]</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.8177355753659387</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[0.1415384163931344, -2.27931078770676]</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>-23.92057657766376</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[0.37000232417084855, -1.8765070025655661]</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.303143234883479</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[0.1531009890234734, -2.3379516315369337]</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>-23.9244338306739</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>[-0.8393213026254611, -1.6459870908884213]</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.142001811702853</v>
+      </c>
+      <c r="H7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[0.10064340760938209, -2.44082582471746]</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>-23.94793308044442</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[-0.3216232578643977, 0.15323874335976545]</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.4566802291950245</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[0.02023759314328266, -2.4025161388775187]</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>-23.95601625894442</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[-0.3952384182991573, 0.9939520939706235]</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.7461873324453905</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[-0.07857201143150666, -2.154028115384863]</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>-23.9814552650821</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>[0.30880972060456374, 0.36020992809542024]</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.4577708801920451</v>
+      </c>
+      <c r="H10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[-0.05927140389372143, -2.131514994878899]</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>-23.98535985929735</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[0.2677219209459053, -0.07239041796487224]</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2515108900369277</v>
+      </c>
+      <c r="H11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[-0.025806163775483268, -2.140563797124508]</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>-23.98828649869769</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[0.27002367758703355, -0.38532158442086206]</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.3051063405989521</v>
+      </c>
+      <c r="H12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>[0.04169975562127512, -2.2368941932297233]</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>-23.99144209861688</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[0.16027003531652095, -0.9825342895371709]</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.4448280394669562</v>
+      </c>
+      <c r="H13" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>[0.05171663282855768, -2.2983025863257964]</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>-23.99175491402846</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[-0.20852006907202256, -0.32396647760099223]</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.2715073621076382</v>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[0.045200380670056974, -2.3084265387508274]</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>-23.99239564321691</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[-0.27071000632799247, -0.05937930207932868]</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1955247573829768</v>
+      </c>
+      <c r="H15" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>[0.028281005274557444, -2.3121377451307854]</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>-23.99303302260687</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[-0.24054002105137823, 0.13368427442477812]</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.192356886139622</v>
+      </c>
+      <c r="H16" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>[0.013247253958846305, -2.3037824779792366]</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>-23.99354016890058</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[-0.294686184056341, 0.4585560391888198]</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.2581035282220587</v>
+      </c>
+      <c r="H17" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>[-0.02358851904819632, -2.246462973080634]</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>-23.99602098677425</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[-0.14482991102755588, 0.7930600843983245]</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.30897409338741</v>
+      </c>
+      <c r="H18" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>[-0.03264038848741856, -2.1968967178057386]</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>-23.99671851056074</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[0.12498424293636826, 0.21883439650589495]</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.1717175680596252</v>
+      </c>
+      <c r="H19" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>[-0.028734630895657056, -2.1900581429149293]</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>-23.99692609763687</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[0.1687822045748053, 0.04553950287510869]</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1242869775082797</v>
+      </c>
+      <c r="H20" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>[-0.018185743109731724, -2.187211923985235]</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>-23.99712650036199</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[0.15289348180426104, -0.07776822650042131]</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.1234291077710573</v>
+      </c>
+      <c r="H21" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>[-0.00862990049696541, -2.1920724381415115]</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>-23.9972751176281</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[0.1918695937827492, -0.28467243910741136]</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.1674954400241539</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>[0.015353798725878241, -2.227656493029938]</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>-23.99816320522331</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>[0.11424643380362531, -0.5422863226071577]</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.2099391359325647</v>
+      </c>
+      <c r="H23" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>[0.022494200838604823, -2.2615493881928854]</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>-23.99846418594047</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[-0.0834195890454796, -0.17600267589294505]</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.1235953112874079</v>
+      </c>
+      <c r="H24" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>[0.019887338680933585, -2.26704947181454]</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>-23.99856732070212</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>[-0.11637595876655595, -0.04303133048692194]</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.08709993585498832</v>
+      </c>
+      <c r="H25" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>[0.012613841258023839, -2.2697389299699724]</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-23.99863586916095</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>[-0.1014039259594827, 0.04357343571995398]</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.08466082173380395</v>
+      </c>
+      <c r="H26" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>[0.006276095885556171, -2.267015590237475]</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>-23.99866446437374</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>[-0.12945035638601635, 0.1805355752575355]</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.1160324903031646</v>
+      </c>
+      <c r="H27" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>[-0.009905198662695873, -2.244448643330283]</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>-23.99903691543783</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>[-0.08785619920741836, 0.38056331580829356]</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.1514133522952789</v>
+      </c>
+      <c r="H28" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>[-0.01539621111315952, -2.2206634360922646]</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>-23.99928886991129</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>[0.05966553149249058, 0.1415185067278382]</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.09234395151326204</v>
+      </c>
+      <c r="H29" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>[-0.013531663254019189, -2.2162409827570198]</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>-23.99937141987164</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>[0.08239449936824067, 0.03740230319968975]</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>0.03125</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.06140902581442672</v>
+      </c>
+      <c r="H30" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>[-0.008382007043504147, -2.213903338807039]</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>-23.99940930400341</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>[0.06208066964298917, -0.024753128758798065]</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.05534244206330603</v>
+      </c>
+      <c r="H31" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>[-0.004501965190817324, -2.215450409354464]</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>-23.99941977161109</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>[0.07520542665902148, -0.10938121925207978]</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.07455167017713681</v>
+      </c>
+      <c r="H32" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>[0.004898713141560361, -2.2291230617609736]</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>-23.99964746473856</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[0.033342669786449064, -0.20752130247249573]</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.09020801205478733</v>
+      </c>
+      <c r="H33" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>[0.006982630003213428, -2.2420931431655045]</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>-23.9998518951588</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>[-0.037098519186760555, -0.057524141979459986]</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.04588574637235277</v>
+      </c>
+      <c r="H34" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>[0.004663972554040894, -2.2456884020392205]</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>-23.99988560924748</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>[-0.016256370631213407, 0.007268696309111524]</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.02143865833750509</v>
+      </c>
+      <c r="H35" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>[0.0005998798962375419, -2.2438712279619426]</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>-23.99989514333731</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>[-0.026636457814850772, 0.051997421324409265]</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.03828802407211161</v>
+      </c>
+      <c r="H36" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>[-0.0027296773306188047, -2.2373715502963916]</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>-23.99994511237183</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>[0.008576999390371834, 0.06285504124630725]</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.03629384272657408</v>
+      </c>
+      <c r="H37" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>[-0.002193614868720565, -2.2334431102184973]</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>-23.99998519220414</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>[0.012307721181163559, 0.004658266645504028]</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.01156604070969202</v>
+      </c>
+      <c r="H38" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>[-0.0006551497210751202, -2.2328608268878094]</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>-23.99998568691943</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>[0.006935210618495722, -0.005207362961320837]</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.01198354650816759</v>
+      </c>
+      <c r="H39" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>[-0.0002216990574191376, -2.233186287072892]</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>-23.99998570144042</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>[0.0003431730221428661, -0.017887962204820775]</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.01413791724149875</v>
+      </c>
+      <c r="H40" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>[-0.00013590580188342107, -2.237658277624097]</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>-23.99999398501504</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>[0.007904444641710306, -0.002695914819586037]</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.01035755675575716</v>
+      </c>
+      <c r="H41" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>[0.0008521497783303672, -2.2379952669765455]</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>-23.99999550967153</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[0.0005990016459567805, 0.003819202202851303]</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.004376608505759047</v>
+      </c>
+      <c r="H42" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>[0.0010019001898195624, -2.2370404664258325]</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>-23.99999698685799</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>[-0.004953882448043662, 0.007375135636990563]</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.006130175169395563</v>
+      </c>
+      <c r="H43" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>[-0.00023657042219135302, -2.2351966825165848]</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>-23.99999902635277</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[-0.002134431745883263, -0.0010278736079142928]</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.002774748666271026</v>
+      </c>
+      <c r="H44" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>[-0.0005033743904267609, -2.235325166717574]</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>-23.9999991251831</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[0.0006289102249102336, -0.0016481166198963788]</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.002274024190713136</v>
+      </c>
+      <c r="H45" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>[-0.00018891927797164414, -2.236149225027522]</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>-23.99999974694831</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>[0.002952459661233077, -0.0008540544075457172]</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.002463827818597342</v>
+      </c>
+      <c r="H46" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>[0.0001801381796824905, -2.2362559818284655]</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>-23.99999990252696</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[-0.0005133132867219705, -0.00012359827994558808]</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.00104983610013207</v>
+      </c>
+      <c r="H47" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Conjugate Gradient</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>[5.1809858001997865e-05, -2.2362868813984518]</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>-23.99999993610638</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>[8.993086290608979e-05, 0.0006039453580112077]</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.0007579875398272995</v>
+      </c>
+      <c r="H48" t="n">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fun</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>grad</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>hesse</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>gnorm</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>iter</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Newton</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>-14</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[8.94427190999916, 8.94427190999916]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>12.64911064067352</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Newton</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[-1.7472540266464002e-17, -2.23606797749979]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-24</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fun</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>grad</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>hesse</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>gnorm</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>iter</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Quasi-Newton</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[0.0, 0.0]</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>-14</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[8.94427190999916, 8.94427190999916]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>12.64911064067352</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Quasi-Newton</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[-1.118033988749895, -1.118033988749895]</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-20.25</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[-6.708203932499369, 0.0]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>6.708203932499369</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Quasi-Newton</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>[-0.07853957772209985, -2.5178864622673256]</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>-23.72177873779113</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[-1.9126697162911412, -1.4414322499585417]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2.395001539631609</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Quasi-Newton</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[0.007156983790086863, -2.212257242967386]</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-23.99792833359288</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>[0.1668127760304845, 0.12387087328996316]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0.207775107981237</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Quasi-Newton</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[-5.751716738305879e-09, -2.2360679698587176]</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>-24</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[-2.6952879039754407e-08, 7.557421355386396e-09]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[[10.0, 4.0], [4.0, 4.0]]</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2.799236156658603e-08</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>